<commit_message>
function to complete logbook data
</commit_message>
<xml_diff>
--- a/inst/extdata/Research_cycle_data_cleaning_logbook_template_v3_202208_FINAL.xlsx
+++ b/inst/extdata/Research_cycle_data_cleaning_logbook_template_v3_202208_FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayana.das\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07F352B7-C087-497B-8318-8AAD68B0CC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C55E8F8-69F3-4F9C-9BDB-527B24EE5455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="20914" r:id="rId7"/>
-    <pivotCache cacheId="20915" r:id="rId8"/>
-    <pivotCache cacheId="20916" r:id="rId9"/>
+    <pivotCache cacheId="1223" r:id="rId7"/>
+    <pivotCache cacheId="1224" r:id="rId8"/>
+    <pivotCache cacheId="1225" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1173,78 +1173,6 @@
       </font>
     </dxf>
     <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -1273,6 +1201,22 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1467,6 +1411,78 @@
       </font>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Roboto Condensed"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -1495,22 +1511,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Roboto Condensed"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -25293,450 +25293,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B8AACB4-921F-4F83-8D88-93370A0D7766}" name="PivotTable6" cacheId="20915" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
-  <location ref="A9:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="12">
-        <item x="6"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Number" fld="0" subtotal="count" baseField="1" baseItem="0"/>
-  </dataFields>
-  <formats count="24">
-    <format dxfId="90">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="91">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="92">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="93">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="94">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="96">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="97">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="99">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="100">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="101">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="102">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="103">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="104">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="105">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="106">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="107">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="108">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="109">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="110">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="111">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="112">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="113">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <conditionalFormats count="2">
-    <conditionalFormat priority="5">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="11">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="8">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="3">
-              <x v="0"/>
-              <x v="2"/>
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50E3D030-46E1-4B1B-BFC0-5288F196554D}" name="PivotTable1" cacheId="20914" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
-  <location ref="M9:N17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="10">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="13">
-        <item m="1" x="9"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item x="1"/>
-        <item m="1" x="7"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item m="1" x="8"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="5" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="27">
-    <format dxfId="63">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="64">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="65">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="66">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
-    </format>
-    <format dxfId="67">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="68">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="69">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="70">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="71">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="72">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="73">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="74">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="75">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
-    </format>
-    <format dxfId="76">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="77">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="78">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="79">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="80">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="81">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="82">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="83">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="84">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
-    </format>
-    <format dxfId="85">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="86">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="87">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="88">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="89">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <conditionalFormats count="2">
-    <conditionalFormat priority="6">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="11">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="13">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="3">
-              <x v="1"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC74FA96-4AC2-4B57-86EE-B23F4684599B}" name="PivotTable5" cacheId="20916" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC74FA96-4AC2-4B57-86EE-B23F4684599B}" name="PivotTable5" cacheId="1225" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
   <location ref="Y9:Z21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -25824,58 +25381,58 @@
     <dataField name="Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="18">
-    <format dxfId="45">
+    <format dxfId="96">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="97">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="98">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="99">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="101">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="102">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="103">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="104">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="105">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="106">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="107">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="108">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="109">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="110">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="111">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -25933,8 +25490,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E38AAB19-7B9A-4206-8225-7D6BE5AEB1ED}" name="PivotTable4" cacheId="20916" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E38AAB19-7B9A-4206-8225-7D6BE5AEB1ED}" name="PivotTable4" cacheId="1225" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
   <location ref="S9:T21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -26008,58 +25565,58 @@
     <dataField name="Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="18">
-    <format dxfId="27">
+    <format dxfId="78">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="79">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="80">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="81">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="84">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="85">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="86">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="87">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="90">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="91">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="92">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="93">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -26118,8 +25675,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB2414D4-EB53-4566-8A70-574BD574110E}" name="PivotTable3" cacheId="20914" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB2414D4-EB53-4566-8A70-574BD574110E}" name="PivotTable3" cacheId="1223" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
   <location ref="G9:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
@@ -26191,6 +25748,449 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Number" fld="0" subtotal="count" baseField="1" baseItem="0"/>
+  </dataFields>
+  <formats count="27">
+    <format dxfId="51">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="52">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="53">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="54">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="55">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="56">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="57">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="59">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="60">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="61">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="62">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="63">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="64">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="65">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="68">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="69">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="70">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="71">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="72">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="73">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="74">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="75">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="77">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <conditionalFormats count="2">
+    <conditionalFormat priority="7">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="11">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="14">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="3">
+              <x v="1"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B8AACB4-921F-4F83-8D88-93370A0D7766}" name="PivotTable6" cacheId="1224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
+  <location ref="A9:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="6"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Number" fld="0" subtotal="count" baseField="1" baseItem="0"/>
+  </dataFields>
+  <formats count="24">
+    <format dxfId="27">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="35">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="36">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="38">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="42">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="43">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="44">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="45">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="46">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="47">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="48">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="49">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="50">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <conditionalFormats count="2">
+    <conditionalFormat priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="11">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="8">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="3">
+              <x v="0"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50E3D030-46E1-4B1B-BFC0-5288F196554D}" name="PivotTable1" cacheId="1223" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Enumerator ID">
+  <location ref="M9:N17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="10">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="13">
+        <item m="1" x="9"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item x="1"/>
+        <item m="1" x="7"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="5" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="27">
     <format dxfId="0">
@@ -26288,7 +26288,7 @@
     </format>
   </formats>
   <conditionalFormats count="2">
-    <conditionalFormat priority="7">
+    <conditionalFormat priority="6">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -26312,7 +26312,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="14">
+    <conditionalFormat priority="13">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -33294,7 +33294,7 @@
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C35" ca="1" si="0">ROUND(RAND()*3,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>75</v>
@@ -33313,7 +33313,7 @@
       </c>
       <c r="C4" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>75</v>
@@ -33351,7 +33351,7 @@
       </c>
       <c r="C6" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>75</v>
@@ -33370,7 +33370,7 @@
       </c>
       <c r="C7" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>75</v>
@@ -33484,7 +33484,7 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>80</v>
@@ -33541,7 +33541,7 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>75</v>
@@ -33578,7 +33578,7 @@
       </c>
       <c r="C18" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>75</v>
@@ -33614,7 +33614,7 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>75</v>
@@ -33632,7 +33632,7 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>75</v>
@@ -33650,7 +33650,7 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>75</v>
@@ -33668,7 +33668,7 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>75</v>
@@ -33704,7 +33704,7 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>75</v>
@@ -33740,7 +33740,7 @@
       </c>
       <c r="C27" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>75</v>
@@ -33758,7 +33758,7 @@
       </c>
       <c r="C28" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>75</v>
@@ -33776,7 +33776,7 @@
       </c>
       <c r="C29" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>82</v>
@@ -33812,7 +33812,7 @@
       </c>
       <c r="C31" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>75</v>
@@ -33830,7 +33830,7 @@
       </c>
       <c r="C32" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>75</v>
@@ -33866,7 +33866,7 @@
       </c>
       <c r="C34" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>84</v>
@@ -33884,7 +33884,7 @@
       </c>
       <c r="C35" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>75</v>

</xml_diff>